<commit_message>
Dawson Analysis and Data cleaning for other neighbourhoods
</commit_message>
<xml_diff>
--- a/Tree_Data/input/MasterSppKey_NativeRegion.xlsx
+++ b/Tree_Data/input/MasterSppKey_NativeRegion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/UltimateGangsta/Documents/GitHub/Trees/Tree_Data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B48B20-97CB-944D-814A-D8D091FE63E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D5083B-D525-D94E-BCFD-9B1996AD4BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7300" yWindow="500" windowWidth="20980" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2946,9 +2946,6 @@
     <t>Amelanchier arborea</t>
   </si>
   <si>
-    <t>Nhttps://www.fs.fed.us/database/feis/plants/tree/amearb/all.htmlA</t>
-  </si>
-  <si>
     <t>AMSA</t>
   </si>
   <si>
@@ -3304,6 +3301,9 @@
   </si>
   <si>
     <t>Abies balsamea</t>
+  </si>
+  <si>
+    <t>https://www.fs.fed.us/database/feis/plants/tree/amearb/all.htmlA</t>
   </si>
 </sst>
 </file>
@@ -20784,8 +20784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E266" sqref="E266"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H270" sqref="H270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20841,7 +20841,7 @@
         <v>724</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>725</v>
@@ -28105,8 +28105,8 @@
       <c r="G267" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="H267" s="37" t="s">
-        <v>973</v>
+      <c r="H267" s="87" t="s">
+        <v>1092</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.2">
@@ -28114,13 +28114,13 @@
         <v>860</v>
       </c>
       <c r="B268" s="37" t="s">
+        <v>973</v>
+      </c>
+      <c r="C268" s="37" t="s">
+        <v>973</v>
+      </c>
+      <c r="D268" s="37" t="s">
         <v>974</v>
-      </c>
-      <c r="C268" s="37" t="s">
-        <v>974</v>
-      </c>
-      <c r="D268" s="37" t="s">
-        <v>975</v>
       </c>
       <c r="E268" s="37"/>
       <c r="F268" s="37" t="s">
@@ -28135,16 +28135,16 @@
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A269" s="37" t="s">
+        <v>975</v>
+      </c>
+      <c r="B269" s="37" t="s">
         <v>976</v>
       </c>
-      <c r="B269" s="37" t="s">
+      <c r="C269" s="37" t="s">
+        <v>976</v>
+      </c>
+      <c r="D269" s="37" t="s">
         <v>977</v>
-      </c>
-      <c r="C269" s="37" t="s">
-        <v>977</v>
-      </c>
-      <c r="D269" s="37" t="s">
-        <v>978</v>
       </c>
       <c r="E269" s="37"/>
       <c r="F269" s="37" t="s">
@@ -28154,21 +28154,21 @@
         <v>9</v>
       </c>
       <c r="H269" s="37" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A270" s="37" t="s">
+        <v>979</v>
+      </c>
+      <c r="B270" s="37" t="s">
         <v>980</v>
       </c>
-      <c r="B270" s="37" t="s">
+      <c r="C270" s="37" t="s">
+        <v>980</v>
+      </c>
+      <c r="D270" s="37" t="s">
         <v>981</v>
-      </c>
-      <c r="C270" s="37" t="s">
-        <v>981</v>
-      </c>
-      <c r="D270" s="37" t="s">
-        <v>982</v>
       </c>
       <c r="E270" s="37"/>
       <c r="F270" s="37" t="s">
@@ -28178,7 +28178,7 @@
         <v>10</v>
       </c>
       <c r="H270" s="37" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.2">
@@ -28186,13 +28186,13 @@
         <v>864</v>
       </c>
       <c r="B271" s="37" t="s">
+        <v>983</v>
+      </c>
+      <c r="C271" s="37" t="s">
+        <v>983</v>
+      </c>
+      <c r="D271" s="37" t="s">
         <v>984</v>
-      </c>
-      <c r="C271" s="37" t="s">
-        <v>984</v>
-      </c>
-      <c r="D271" s="37" t="s">
-        <v>985</v>
       </c>
       <c r="E271" s="37"/>
       <c r="F271" s="37" t="s">
@@ -28202,7 +28202,7 @@
         <v>10</v>
       </c>
       <c r="H271" s="37" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.2">
@@ -28210,13 +28210,13 @@
         <v>864</v>
       </c>
       <c r="B272" s="37" t="s">
+        <v>986</v>
+      </c>
+      <c r="C272" s="37" t="s">
+        <v>986</v>
+      </c>
+      <c r="D272" s="37" t="s">
         <v>987</v>
-      </c>
-      <c r="C272" s="37" t="s">
-        <v>987</v>
-      </c>
-      <c r="D272" s="37" t="s">
-        <v>988</v>
       </c>
       <c r="E272" s="37"/>
       <c r="F272" s="37" t="s">
@@ -28234,13 +28234,13 @@
         <v>873</v>
       </c>
       <c r="B273" s="37" t="s">
+        <v>988</v>
+      </c>
+      <c r="C273" s="37" t="s">
+        <v>988</v>
+      </c>
+      <c r="D273" s="37" t="s">
         <v>989</v>
-      </c>
-      <c r="C273" s="37" t="s">
-        <v>989</v>
-      </c>
-      <c r="D273" s="37" t="s">
-        <v>990</v>
       </c>
       <c r="E273" s="37"/>
       <c r="F273" s="37" t="s">
@@ -28250,7 +28250,7 @@
         <v>9</v>
       </c>
       <c r="H273" s="37" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.2">
@@ -28258,10 +28258,10 @@
         <v>881</v>
       </c>
       <c r="B274" s="37" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C274" s="37" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D274" s="37" t="s">
         <v>198</v>
@@ -28274,7 +28274,7 @@
         <v>9</v>
       </c>
       <c r="H274" s="37" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.2">
@@ -28282,13 +28282,13 @@
         <v>881</v>
       </c>
       <c r="B275" s="37" t="s">
+        <v>993</v>
+      </c>
+      <c r="C275" s="37" t="s">
+        <v>993</v>
+      </c>
+      <c r="D275" s="37" t="s">
         <v>994</v>
-      </c>
-      <c r="C275" s="37" t="s">
-        <v>994</v>
-      </c>
-      <c r="D275" s="37" t="s">
-        <v>995</v>
       </c>
       <c r="E275" s="37"/>
       <c r="F275" s="37" t="s">
@@ -28306,13 +28306,13 @@
         <v>881</v>
       </c>
       <c r="B276" s="37" t="s">
+        <v>995</v>
+      </c>
+      <c r="C276" s="37" t="s">
+        <v>995</v>
+      </c>
+      <c r="D276" s="37" t="s">
         <v>996</v>
-      </c>
-      <c r="C276" s="37" t="s">
-        <v>996</v>
-      </c>
-      <c r="D276" s="37" t="s">
-        <v>997</v>
       </c>
       <c r="E276" s="37"/>
       <c r="F276" s="37" t="s">
@@ -28322,21 +28322,21 @@
         <v>10</v>
       </c>
       <c r="H276" s="37" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A277" s="37" t="s">
+        <v>998</v>
+      </c>
+      <c r="B277" s="37" t="s">
+        <v>998</v>
+      </c>
+      <c r="C277" s="37" t="s">
+        <v>998</v>
+      </c>
+      <c r="D277" s="37" t="s">
         <v>999</v>
-      </c>
-      <c r="B277" s="37" t="s">
-        <v>999</v>
-      </c>
-      <c r="C277" s="37" t="s">
-        <v>999</v>
-      </c>
-      <c r="D277" s="37" t="s">
-        <v>1000</v>
       </c>
       <c r="E277" s="37"/>
       <c r="F277" s="37" t="s">
@@ -28351,16 +28351,16 @@
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A278" s="37" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B278" s="37" t="s">
         <v>1001</v>
       </c>
-      <c r="B278" s="37" t="s">
+      <c r="C278" s="37" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D278" s="37" t="s">
         <v>1002</v>
-      </c>
-      <c r="C278" s="37" t="s">
-        <v>1002</v>
-      </c>
-      <c r="D278" s="37" t="s">
-        <v>1003</v>
       </c>
       <c r="E278" s="37"/>
       <c r="F278" s="37" t="s">
@@ -28370,21 +28370,21 @@
         <v>10</v>
       </c>
       <c r="H278" s="87" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279" s="37" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B279" s="37" t="s">
         <v>1005</v>
       </c>
-      <c r="B279" s="37" t="s">
+      <c r="C279" s="37" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D279" s="37" t="s">
         <v>1006</v>
-      </c>
-      <c r="C279" s="37" t="s">
-        <v>1006</v>
-      </c>
-      <c r="D279" s="37" t="s">
-        <v>1007</v>
       </c>
       <c r="E279" s="37"/>
       <c r="F279" s="37" t="s">
@@ -28394,7 +28394,7 @@
         <v>10</v>
       </c>
       <c r="H279" s="37" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.2">
@@ -28408,7 +28408,7 @@
         <v>889</v>
       </c>
       <c r="D280" s="37" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="E280" s="37"/>
       <c r="F280" s="37" t="s">
@@ -28426,13 +28426,13 @@
         <v>889</v>
       </c>
       <c r="B281" s="37" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C281" s="37" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D281" s="37" t="s">
         <v>1010</v>
-      </c>
-      <c r="C281" s="37" t="s">
-        <v>1010</v>
-      </c>
-      <c r="D281" s="37" t="s">
-        <v>1011</v>
       </c>
       <c r="E281" s="37"/>
       <c r="F281" s="37" t="s">
@@ -28442,7 +28442,7 @@
         <v>9</v>
       </c>
       <c r="H281" s="37" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.2">
@@ -28450,13 +28450,13 @@
         <v>891</v>
       </c>
       <c r="B282" s="37" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C282" s="37" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D282" s="37" t="s">
         <v>1013</v>
-      </c>
-      <c r="C282" s="37" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D282" s="37" t="s">
-        <v>1014</v>
       </c>
       <c r="E282" s="37"/>
       <c r="F282" s="37" t="s">
@@ -28466,7 +28466,7 @@
         <v>9</v>
       </c>
       <c r="H282" s="37" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.2">
@@ -28474,13 +28474,13 @@
         <v>894</v>
       </c>
       <c r="B283" s="37" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C283" s="37" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D283" s="37" t="s">
         <v>1016</v>
-      </c>
-      <c r="C283" s="37" t="s">
-        <v>1016</v>
-      </c>
-      <c r="D283" s="37" t="s">
-        <v>1017</v>
       </c>
       <c r="E283" s="37"/>
       <c r="F283" s="37" t="s">
@@ -28490,7 +28490,7 @@
         <v>10</v>
       </c>
       <c r="H283" s="37" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.2">
@@ -28498,13 +28498,13 @@
         <v>895</v>
       </c>
       <c r="B284" s="37" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C284" s="37" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D284" s="37" t="s">
         <v>1019</v>
-      </c>
-      <c r="C284" s="37" t="s">
-        <v>1019</v>
-      </c>
-      <c r="D284" s="37" t="s">
-        <v>1020</v>
       </c>
       <c r="E284" s="37"/>
       <c r="F284" s="37" t="s">
@@ -28514,7 +28514,7 @@
         <v>10</v>
       </c>
       <c r="H284" s="37" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.2">
@@ -28522,13 +28522,13 @@
         <v>899</v>
       </c>
       <c r="B285" s="37" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C285" s="37" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D285" s="37" t="s">
         <v>1022</v>
-      </c>
-      <c r="C285" s="37" t="s">
-        <v>1022</v>
-      </c>
-      <c r="D285" s="37" t="s">
-        <v>1023</v>
       </c>
       <c r="E285" s="37"/>
       <c r="F285" s="37" t="s">
@@ -28552,7 +28552,7 @@
         <v>899</v>
       </c>
       <c r="D286" s="37" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="E286" s="37"/>
       <c r="F286" s="37" t="s">
@@ -28570,13 +28570,13 @@
         <v>899</v>
       </c>
       <c r="B287" s="37" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C287" s="37" t="s">
         <v>1025</v>
       </c>
-      <c r="C287" s="37" t="s">
+      <c r="D287" s="37" t="s">
         <v>1026</v>
-      </c>
-      <c r="D287" s="37" t="s">
-        <v>1027</v>
       </c>
       <c r="E287" s="37"/>
       <c r="F287" s="37" t="s">
@@ -28594,13 +28594,13 @@
         <v>899</v>
       </c>
       <c r="B288" s="37" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C288" s="37" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D288" s="37" t="s">
         <v>1028</v>
-      </c>
-      <c r="C288" s="37" t="s">
-        <v>1028</v>
-      </c>
-      <c r="D288" s="37" t="s">
-        <v>1029</v>
       </c>
       <c r="E288" s="37"/>
       <c r="F288" s="37" t="s">
@@ -28618,13 +28618,13 @@
         <v>899</v>
       </c>
       <c r="B289" s="37" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C289" s="37" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D289" s="37" t="s">
         <v>1030</v>
-      </c>
-      <c r="C289" s="37" t="s">
-        <v>1030</v>
-      </c>
-      <c r="D289" s="37" t="s">
-        <v>1031</v>
       </c>
       <c r="E289" s="37"/>
       <c r="F289" s="37" t="s">
@@ -28634,7 +28634,7 @@
         <v>9</v>
       </c>
       <c r="H289" s="37" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.2">
@@ -28642,13 +28642,13 @@
         <v>899</v>
       </c>
       <c r="B290" s="37" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C290" s="37" t="s">
         <v>1033</v>
       </c>
-      <c r="C290" s="37" t="s">
+      <c r="D290" s="37" t="s">
         <v>1034</v>
-      </c>
-      <c r="D290" s="37" t="s">
-        <v>1035</v>
       </c>
       <c r="E290" s="37"/>
       <c r="F290" s="37" t="s">
@@ -28666,13 +28666,13 @@
         <v>899</v>
       </c>
       <c r="B291" s="37" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C291" s="37" t="s">
         <v>1036</v>
       </c>
-      <c r="C291" s="37" t="s">
+      <c r="D291" s="37" t="s">
         <v>1037</v>
-      </c>
-      <c r="D291" s="37" t="s">
-        <v>1038</v>
       </c>
       <c r="E291" s="37"/>
       <c r="F291" s="37" t="s">
@@ -28690,13 +28690,13 @@
         <v>904</v>
       </c>
       <c r="B292" s="37" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C292" s="37" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D292" s="37" t="s">
         <v>1039</v>
-      </c>
-      <c r="C292" s="37" t="s">
-        <v>1039</v>
-      </c>
-      <c r="D292" s="37" t="s">
-        <v>1040</v>
       </c>
       <c r="E292" s="37"/>
       <c r="F292" s="37" t="s">
@@ -28706,7 +28706,7 @@
         <v>9</v>
       </c>
       <c r="H292" s="37" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.2">
@@ -28714,13 +28714,13 @@
         <v>908</v>
       </c>
       <c r="B293" s="37" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C293" s="37" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D293" s="37" t="s">
         <v>1042</v>
-      </c>
-      <c r="C293" s="37" t="s">
-        <v>1042</v>
-      </c>
-      <c r="D293" s="37" t="s">
-        <v>1043</v>
       </c>
       <c r="E293" s="37"/>
       <c r="F293" s="37" t="s">
@@ -28730,7 +28730,7 @@
         <v>9</v>
       </c>
       <c r="H293" s="37" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.2">
@@ -28738,13 +28738,13 @@
         <v>913</v>
       </c>
       <c r="B294" s="37" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C294" s="37" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D294" s="37" t="s">
         <v>1045</v>
-      </c>
-      <c r="C294" s="37" t="s">
-        <v>1045</v>
-      </c>
-      <c r="D294" s="37" t="s">
-        <v>1046</v>
       </c>
       <c r="E294" s="37"/>
       <c r="F294" s="37" t="s">
@@ -28768,7 +28768,7 @@
         <v>914</v>
       </c>
       <c r="D295" s="37" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E295" s="37"/>
       <c r="F295" s="37" t="s">
@@ -28786,13 +28786,13 @@
         <v>921</v>
       </c>
       <c r="B296" s="37" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C296" s="37" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D296" s="37" t="s">
         <v>1048</v>
-      </c>
-      <c r="C296" s="37" t="s">
-        <v>1048</v>
-      </c>
-      <c r="D296" s="37" t="s">
-        <v>1049</v>
       </c>
       <c r="E296" s="37"/>
       <c r="F296" s="37" t="s">
@@ -28802,7 +28802,7 @@
         <v>9</v>
       </c>
       <c r="H296" s="37" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.2">
@@ -28810,13 +28810,13 @@
         <v>921</v>
       </c>
       <c r="B297" s="37" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C297" s="37" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D297" s="37" t="s">
         <v>1051</v>
-      </c>
-      <c r="C297" s="37" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D297" s="37" t="s">
-        <v>1052</v>
       </c>
       <c r="E297" s="37"/>
       <c r="F297" s="37" t="s">
@@ -28826,7 +28826,7 @@
         <v>9</v>
       </c>
       <c r="H297" s="37" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="298" spans="1:8" x14ac:dyDescent="0.2">
@@ -28834,13 +28834,13 @@
         <v>921</v>
       </c>
       <c r="B298" s="37" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C298" s="37" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D298" s="37" t="s">
         <v>1054</v>
-      </c>
-      <c r="C298" s="37" t="s">
-        <v>1054</v>
-      </c>
-      <c r="D298" s="37" t="s">
-        <v>1055</v>
       </c>
       <c r="E298" s="37"/>
       <c r="F298" s="37" t="s">
@@ -28850,7 +28850,7 @@
         <v>9</v>
       </c>
       <c r="H298" s="37" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.2">
@@ -28858,13 +28858,13 @@
         <v>922</v>
       </c>
       <c r="B299" s="37" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C299" s="37" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D299" s="37" t="s">
         <v>1057</v>
-      </c>
-      <c r="C299" s="37" t="s">
-        <v>1057</v>
-      </c>
-      <c r="D299" s="37" t="s">
-        <v>1058</v>
       </c>
       <c r="E299" s="37"/>
       <c r="F299" s="37" t="s">
@@ -28874,7 +28874,7 @@
         <v>10</v>
       </c>
       <c r="H299" s="87" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.2">
@@ -28882,13 +28882,13 @@
         <v>927</v>
       </c>
       <c r="B300" s="37" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C300" s="37" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D300" s="37" t="s">
         <v>1060</v>
-      </c>
-      <c r="C300" s="37" t="s">
-        <v>1060</v>
-      </c>
-      <c r="D300" s="37" t="s">
-        <v>1061</v>
       </c>
       <c r="E300" s="37"/>
       <c r="F300" s="37" t="s">
@@ -28898,7 +28898,7 @@
         <v>10</v>
       </c>
       <c r="H300" s="37" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.2">
@@ -28906,13 +28906,13 @@
         <v>927</v>
       </c>
       <c r="B301" s="37" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C301" s="37" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D301" s="37" t="s">
         <v>1063</v>
-      </c>
-      <c r="C301" s="37" t="s">
-        <v>1063</v>
-      </c>
-      <c r="D301" s="37" t="s">
-        <v>1064</v>
       </c>
       <c r="E301" s="37"/>
       <c r="F301" s="37" t="s">
@@ -28930,13 +28930,13 @@
         <v>930</v>
       </c>
       <c r="B302" s="37" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C302" s="37" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D302" s="37" t="s">
         <v>1065</v>
-      </c>
-      <c r="C302" s="37" t="s">
-        <v>1065</v>
-      </c>
-      <c r="D302" s="37" t="s">
-        <v>1066</v>
       </c>
       <c r="E302" s="37"/>
       <c r="F302" s="37" t="s">
@@ -28946,7 +28946,7 @@
         <v>9</v>
       </c>
       <c r="H302" s="37" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.2">
@@ -28954,13 +28954,13 @@
         <v>930</v>
       </c>
       <c r="B303" s="37" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C303" s="37" t="s">
         <v>1068</v>
       </c>
-      <c r="C303" s="37" t="s">
+      <c r="D303" s="37" t="s">
         <v>1069</v>
-      </c>
-      <c r="D303" s="37" t="s">
-        <v>1070</v>
       </c>
       <c r="E303" s="37"/>
       <c r="F303" s="37" t="s">
@@ -28970,7 +28970,7 @@
         <v>10</v>
       </c>
       <c r="H303" s="37" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.2">
@@ -28978,13 +28978,13 @@
         <v>931</v>
       </c>
       <c r="B304" s="37" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C304" s="37" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D304" s="37" t="s">
         <v>1072</v>
-      </c>
-      <c r="C304" s="37" t="s">
-        <v>1072</v>
-      </c>
-      <c r="D304" s="37" t="s">
-        <v>1073</v>
       </c>
       <c r="E304" s="37"/>
       <c r="F304" s="37" t="s">
@@ -28994,7 +28994,7 @@
         <v>10</v>
       </c>
       <c r="H304" s="37" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.2">
@@ -29008,7 +29008,7 @@
         <v>938</v>
       </c>
       <c r="D305" s="37" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E305" s="37"/>
       <c r="F305" s="37" t="s">
@@ -29026,13 +29026,13 @@
         <v>938</v>
       </c>
       <c r="B306" s="37" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C306" s="37" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D306" s="37" t="s">
         <v>1076</v>
-      </c>
-      <c r="C306" s="37" t="s">
-        <v>1076</v>
-      </c>
-      <c r="D306" s="37" t="s">
-        <v>1077</v>
       </c>
       <c r="E306" s="37"/>
       <c r="F306" s="37" t="s">
@@ -29042,7 +29042,7 @@
         <v>10</v>
       </c>
       <c r="H306" s="37" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.2">
@@ -29050,13 +29050,13 @@
         <v>938</v>
       </c>
       <c r="B307" s="37" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C307" s="37" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D307" s="37" t="s">
         <v>1079</v>
-      </c>
-      <c r="C307" s="37" t="s">
-        <v>1079</v>
-      </c>
-      <c r="D307" s="37" t="s">
-        <v>1080</v>
       </c>
       <c r="E307" s="37"/>
       <c r="F307" s="37" t="s">
@@ -29066,7 +29066,7 @@
         <v>9</v>
       </c>
       <c r="H307" s="37" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.2">
@@ -29074,13 +29074,13 @@
         <v>938</v>
       </c>
       <c r="B308" s="37" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C308" s="37" t="s">
         <v>1082</v>
       </c>
-      <c r="C308" s="37" t="s">
+      <c r="D308" s="37" t="s">
         <v>1083</v>
-      </c>
-      <c r="D308" s="37" t="s">
-        <v>1084</v>
       </c>
       <c r="E308" s="37"/>
       <c r="F308" s="37" t="s">
@@ -29098,13 +29098,13 @@
         <v>938</v>
       </c>
       <c r="B309" s="37" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C309" s="37" t="s">
         <v>1085</v>
       </c>
-      <c r="C309" s="37" t="s">
+      <c r="D309" s="37" t="s">
         <v>1086</v>
-      </c>
-      <c r="D309" s="37" t="s">
-        <v>1087</v>
       </c>
       <c r="E309" s="37"/>
       <c r="F309" s="37" t="s">
@@ -29122,13 +29122,13 @@
         <v>949</v>
       </c>
       <c r="B310" s="37" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C310" s="37" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D310" s="37" t="s">
         <v>1088</v>
-      </c>
-      <c r="C310" s="37" t="s">
-        <v>1088</v>
-      </c>
-      <c r="D310" s="37" t="s">
-        <v>1089</v>
       </c>
       <c r="E310" s="37"/>
       <c r="F310" s="37" t="s">
@@ -29138,7 +29138,7 @@
         <v>9</v>
       </c>
       <c r="H310" s="37" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.2">
@@ -29152,7 +29152,7 @@
         <v>816</v>
       </c>
       <c r="D311" s="37" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E311" s="37"/>
       <c r="F311" s="37" t="s">
@@ -29171,9 +29171,10 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="H143" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H267" r:id="rId2" xr:uid="{887202F5-6672-8C47-A57C-9082F6B89854}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>